<commit_message>
Apply EXP() back-transformation to species models.  Update example files, recompile installer.
git-svn-id: http://Marc-PC/svn/Full@3775 85f15e0e-5137-b144-a863-98bd542365a3
</commit_message>
<xml_diff>
--- a/trunk/output-bird-habitat/branches/century/tests/bird_model_test_transform.xlsx
+++ b/trunk/output-bird-habitat/branches/century/tests/bird_model_test_transform.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="8415" yWindow="45" windowWidth="17235" windowHeight="7995" activeTab="2"/>
+    <workbookView xWindow="-540" yWindow="375" windowWidth="17235" windowHeight="7995" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="PIWA" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="33">
   <si>
     <t>int</t>
   </si>
@@ -103,6 +103,18 @@
   </si>
   <si>
     <t>Biomass</t>
+  </si>
+  <si>
+    <t>Test2</t>
+  </si>
+  <si>
+    <t>MinPrecip</t>
+  </si>
+  <si>
+    <t>MaxPrecip</t>
+  </si>
+  <si>
+    <t>12.95 in output</t>
   </si>
 </sst>
 </file>
@@ -249,7 +261,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -427,6 +439,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -599,7 +617,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -626,6 +644,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -635,7 +660,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -978,10 +1006,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A20" sqref="A20:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -991,12 +1019,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
       <c r="I1" s="8"/>
@@ -1144,33 +1172,33 @@
       <c r="K9" s="9"/>
     </row>
     <row r="10" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="21"/>
     </row>
     <row r="11" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
       <c r="E11" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G11" s="10"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="21"/>
       <c r="K11" s="10"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1207,9 +1235,9 @@
         <f>E6</f>
         <v>99.28</v>
       </c>
-      <c r="E13">
-        <f>B$4+B13*C$4+C13*D$4+D13*E$4</f>
-        <v>102.58608776998369</v>
+      <c r="E13" s="6">
+        <f t="shared" ref="E13:E18" si="1">EXP(B$3+B13*C$3+C13*D$3+D13*E$3)</f>
+        <v>0.4523375925268675</v>
       </c>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
@@ -1233,8 +1261,8 @@
         <v>99.28</v>
       </c>
       <c r="E14" s="6">
-        <f t="shared" ref="E14:E18" si="1">B$4+B14*C$4+C14*D$4+D14*E$4</f>
-        <v>108.15686846212301</v>
+        <f t="shared" si="1"/>
+        <v>0.13528204715127137</v>
       </c>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
@@ -1259,7 +1287,7 @@
       </c>
       <c r="E15" s="6">
         <f t="shared" si="1"/>
-        <v>103.60251249663909</v>
+        <v>2.6082711337498406E-2</v>
       </c>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
@@ -1284,7 +1312,7 @@
       </c>
       <c r="E16" s="6">
         <f t="shared" si="1"/>
-        <v>108.15686846212301</v>
+        <v>0.13528204715127137</v>
       </c>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
@@ -1309,7 +1337,7 @@
       </c>
       <c r="E17" s="6">
         <f t="shared" si="1"/>
-        <v>7.1066330093898191</v>
+        <v>1.7265095585019787E-2</v>
       </c>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
@@ -1334,7 +1362,7 @@
       </c>
       <c r="E18" s="6">
         <f t="shared" si="1"/>
-        <v>108.15686846212301</v>
+        <v>0.13528204715127137</v>
       </c>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
@@ -1347,23 +1375,41 @@
         <v>25</v>
       </c>
       <c r="B19" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C19" s="6">
-        <v>3.43</v>
+        <v>1.31</v>
       </c>
       <c r="D19" s="6">
         <v>100</v>
       </c>
       <c r="E19" s="6">
         <f t="shared" ref="E19" si="2">B$4+B19*C$4+C19*D$4+D19*E$4</f>
-        <v>109.52696642989248</v>
+        <v>103.2005391473749</v>
       </c>
       <c r="G19" s="11"/>
       <c r="H19" s="11"/>
       <c r="I19" s="11"/>
       <c r="J19" s="11"/>
       <c r="K19" s="11"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="22">
+        <v>0</v>
+      </c>
+      <c r="C20" s="22">
+        <v>1.31</v>
+      </c>
+      <c r="D20" s="22">
+        <v>100</v>
+      </c>
+      <c r="E20" s="24">
+        <f>EXP(B$3+B20*C$3+C20*D$3+D20*E$3)</f>
+        <v>3.3873592854351216E-2</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1383,7 +1429,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1"/>
+      <selection activeCell="A15" sqref="A15:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1395,10 +1441,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="16"/>
+      <c r="C1" s="19"/>
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
@@ -1523,16 +1569,16 @@
       <c r="J9" s="12"/>
     </row>
     <row r="10" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
       <c r="J10" s="12"/>
     </row>
     <row r="11" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1543,9 +1589,9 @@
       <c r="C11" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="10"/>
       <c r="H11" s="12"/>
     </row>
@@ -1572,7 +1618,7 @@
         <v>0</v>
       </c>
       <c r="C13" s="6">
-        <f>B$4+B13*C$4</f>
+        <f>EXP(B$3+B13*C$3)</f>
         <v>5.0612084504354105E-3</v>
       </c>
       <c r="D13" s="8"/>
@@ -1590,8 +1636,8 @@
         <v>2.0043213737826426</v>
       </c>
       <c r="C14" s="6">
-        <f t="shared" ref="C14" si="0">B$4+B14*C$4</f>
-        <v>5.3175240331601143</v>
+        <f>EXP(B$3+B14*C$3)</f>
+        <v>3.5705957016643114E-2</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
@@ -1600,6 +1646,16 @@
       <c r="H14" s="11"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="22">
+        <v>0</v>
+      </c>
+      <c r="C15" s="24">
+        <f>EXP(B$3+B15*C$3)</f>
+        <v>5.0612084504354105E-3</v>
+      </c>
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
@@ -1621,27 +1677,30 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="9.140625" style="6"/>
+    <col min="2" max="2" width="9.140625" style="6"/>
+    <col min="3" max="4" width="14.7109375" style="6" customWidth="1"/>
+    <col min="5" max="6" width="9.140625" style="6"/>
     <col min="7" max="7" width="23" style="6" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
       <c r="I1" s="8"/>
@@ -1649,19 +1708,19 @@
       <c r="K1" s="8"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="18" t="s">
         <v>28</v>
       </c>
       <c r="G2" s="8"/>
@@ -1674,11 +1733,21 @@
       <c r="A3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="19">
-        <v>0.20618117632497523</v>
-      </c>
-      <c r="C3" s="19">
-        <v>0.77724473806894612</v>
+      <c r="B3" s="16">
+        <v>-1.579</v>
+      </c>
+      <c r="C3" s="16">
+        <v>-0.252</v>
+      </c>
+      <c r="D3" s="16">
+        <v>0.2732</v>
+      </c>
+      <c r="E3" s="23">
+        <f t="shared" ref="C3:F3" si="0">LN(E4)</f>
+        <v>2.0430000000000101E-2</v>
+      </c>
+      <c r="F3" s="25">
+        <v>5.8819999999999998E-6</v>
       </c>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
@@ -1690,21 +1759,19 @@
       <c r="A4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="6">
-        <f>EXP(B3)</f>
-        <v>1.2289758451531578</v>
-      </c>
-      <c r="C4" s="6">
-        <f t="shared" ref="C4" si="0">EXP(C3)</f>
-        <v>2.1754700107006562</v>
-      </c>
-      <c r="D4" s="19">
+      <c r="B4" s="16">
+        <v>0.20618117632497523</v>
+      </c>
+      <c r="C4" s="16">
+        <v>0.77724473806894612</v>
+      </c>
+      <c r="D4" s="16">
         <v>1.314163051153461</v>
       </c>
-      <c r="E4" s="19">
+      <c r="E4" s="16">
         <v>1.0206401209341016</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F4" s="16">
         <v>1.000005882017299</v>
       </c>
       <c r="G4" s="8"/>
@@ -1759,6 +1826,10 @@
         <f>LOG(C5+1)</f>
         <v>0</v>
       </c>
+      <c r="D7" s="6">
+        <f>LOG(D5+1)</f>
+        <v>1.5485429604650471</v>
+      </c>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
@@ -1772,6 +1843,10 @@
       <c r="C8" s="6">
         <f>LOG(C6+1)</f>
         <v>1.9987822698317359</v>
+      </c>
+      <c r="D8" s="6">
+        <f>LOG(D6+1)</f>
+        <v>2.1163154597653446</v>
       </c>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
@@ -1787,53 +1862,53 @@
       <c r="K9" s="9"/>
     </row>
     <row r="10" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="21"/>
     </row>
     <row r="11" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14"/>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="14"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
       <c r="F11" s="14" t="s">
         <v>14</v>
       </c>
       <c r="H11" s="15"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="21"/>
       <c r="L11" s="15"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="str">
+      <c r="B12" s="17" t="str">
         <f>C2</f>
         <v>LogUC200</v>
       </c>
-      <c r="C12" s="1" t="str">
+      <c r="C12" s="17" t="str">
         <f>D2</f>
         <v>LogPrevPrecip</v>
       </c>
-      <c r="D12" s="1" t="str">
+      <c r="D12" s="17" t="str">
         <f>E2</f>
         <v>UF500</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="17" t="s">
         <v>27</v>
       </c>
       <c r="H12" s="8"/>
@@ -1844,15 +1919,15 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B13" s="6">
         <f>C8</f>
         <v>1.9987822698317359</v>
       </c>
       <c r="C13" s="6">
-        <f>D5</f>
-        <v>34.362499999999997</v>
+        <f>D7</f>
+        <v>1.5485429604650471</v>
       </c>
       <c r="D13" s="6">
         <f>E6</f>
@@ -1862,8 +1937,8 @@
         <v>1000</v>
       </c>
       <c r="F13" s="6">
-        <f>B$4+B13*C$4+C13*D$4+D13*E$4+E13*F$4</f>
-        <v>1152.0702277999897</v>
+        <f t="shared" ref="F13:F18" si="1">EXP(B$3+B13*C$3+C13*D$3+D13*E$3+E13*F$3)</f>
+        <v>1.4543240246526252</v>
       </c>
       <c r="H13" s="8"/>
       <c r="I13" s="8"/>
@@ -1873,15 +1948,15 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="B14" s="6">
         <f>C8</f>
         <v>1.9987822698317359</v>
       </c>
       <c r="C14" s="6">
-        <f>D6</f>
-        <v>129.71199999999999</v>
+        <f>D8</f>
+        <v>2.1163154597653446</v>
       </c>
       <c r="D14" s="6">
         <f>E6</f>
@@ -1891,8 +1966,8 @@
         <v>1000</v>
       </c>
       <c r="F14" s="6">
-        <f t="shared" ref="F14:F19" si="1">B$4+B14*C$4+C14*D$4+D14*E$4+E14*F$4</f>
-        <v>1277.3750176459466</v>
+        <f t="shared" si="1"/>
+        <v>1.6983490830766903</v>
       </c>
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
@@ -1909,7 +1984,7 @@
         <v>0</v>
       </c>
       <c r="C15" s="6">
-        <v>2.6724999999999999</v>
+        <v>2.1163154597653446</v>
       </c>
       <c r="D15" s="6">
         <f>E6</f>
@@ -1920,7 +1995,7 @@
       </c>
       <c r="F15" s="6">
         <f t="shared" si="1"/>
-        <v>1106.0761098229973</v>
+        <v>2.8104645321295001</v>
       </c>
       <c r="H15" s="8"/>
       <c r="I15" s="8"/>
@@ -1937,7 +2012,7 @@
         <v>1.9987822698317359</v>
       </c>
       <c r="C16" s="6">
-        <v>2.6724999999999999</v>
+        <v>2.1163154597653446</v>
       </c>
       <c r="D16" s="6">
         <f>E6</f>
@@ -1948,7 +2023,7 @@
       </c>
       <c r="F16" s="6">
         <f t="shared" si="1"/>
-        <v>1110.4244007089364</v>
+        <v>1.6983490830766903</v>
       </c>
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
@@ -1965,7 +2040,7 @@
         <v>1.9987822698317359</v>
       </c>
       <c r="C17" s="6">
-        <v>2.6724999999999999</v>
+        <v>2.1163154597653446</v>
       </c>
       <c r="D17" s="6">
         <f>E5</f>
@@ -1976,7 +2051,7 @@
       </c>
       <c r="F17" s="6">
         <f t="shared" si="1"/>
-        <v>1009.4116479400884</v>
+        <v>0.2248547932630193</v>
       </c>
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
@@ -1993,7 +2068,7 @@
         <v>1.9987822698317359</v>
       </c>
       <c r="C18" s="6">
-        <v>2.6724999999999999</v>
+        <v>2.1163154597653446</v>
       </c>
       <c r="D18" s="6">
         <f>E6</f>
@@ -2004,7 +2079,7 @@
       </c>
       <c r="F18" s="6">
         <f t="shared" si="1"/>
-        <v>1110.4244007089364</v>
+        <v>1.6983490830766903</v>
       </c>
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
@@ -2020,17 +2095,17 @@
         <v>0</v>
       </c>
       <c r="C19" s="6">
-        <v>6.62</v>
+        <v>3.9309430000000001</v>
       </c>
       <c r="D19" s="6">
         <v>100</v>
       </c>
       <c r="E19" s="6">
-        <v>11084</v>
+        <v>10965</v>
       </c>
       <c r="F19" s="6">
-        <f t="shared" si="1"/>
-        <v>11196.057943616941</v>
+        <f>B$4+B19*C$4+C19*D$4+D19*E$4+E19*F$4</f>
+        <v>11072.500589636209</v>
       </c>
       <c r="H19" s="11"/>
       <c r="I19" s="11"/>
@@ -2038,13 +2113,37 @@
       <c r="K19" s="11"/>
       <c r="L19" s="11"/>
     </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="22">
+        <v>0</v>
+      </c>
+      <c r="C20" s="22">
+        <v>7.46</v>
+      </c>
+      <c r="D20" s="22">
+        <v>100</v>
+      </c>
+      <c r="E20" s="22">
+        <v>10965</v>
+      </c>
+      <c r="F20" s="24">
+        <f>EXP(B$3+B20*C$3+C20*D$3+D20*E$3+E20*F$3)</f>
+        <v>13.021061084954049</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="B1:E1"/>
     <mergeCell ref="A10:E10"/>
     <mergeCell ref="G10:K10"/>
-    <mergeCell ref="B11:D11"/>
     <mergeCell ref="I11:K11"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B11:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>